<commit_message>
cwl june 2025 roster
</commit_message>
<xml_diff>
--- a/xray-members.xlsx
+++ b/xray-members.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="313">
   <si>
     <t>DisplayName</t>
   </si>
@@ -202,6 +202,18 @@
     <t>#8CLR9YULP</t>
   </si>
   <si>
+    <t>TheHive</t>
+  </si>
+  <si>
+    <t>thehive1985</t>
+  </si>
+  <si>
+    <t>463802886879445024</t>
+  </si>
+  <si>
+    <t>#GRRUUC8V9</t>
+  </si>
+  <si>
     <t>Mori-san</t>
   </si>
   <si>
@@ -403,45 +415,6 @@
     <t>#90ULVLUC</t>
   </si>
   <si>
-    <t>dhruba</t>
-  </si>
-  <si>
-    <t>roronoazoro5075</t>
-  </si>
-  <si>
-    <t>1054828813248376883</t>
-  </si>
-  <si>
-    <t>dhruba.</t>
-  </si>
-  <si>
-    <t>#Y89GC9PR8</t>
-  </si>
-  <si>
-    <t>Dhurba</t>
-  </si>
-  <si>
-    <t>#YP2UQJLYL</t>
-  </si>
-  <si>
-    <t>danger gamer</t>
-  </si>
-  <si>
-    <t>#Y2YPGQU2J</t>
-  </si>
-  <si>
-    <t>danger gamer 4</t>
-  </si>
-  <si>
-    <t>#Q2U98U0YY</t>
-  </si>
-  <si>
-    <t>Taco Tornado</t>
-  </si>
-  <si>
-    <t>#LPQCPYR0P</t>
-  </si>
-  <si>
     <t>Protips</t>
   </si>
   <si>
@@ -472,6 +445,18 @@
     <t>#CVYG8LU</t>
   </si>
   <si>
+    <t>Carsonn</t>
+  </si>
+  <si>
+    <t>carson07794</t>
+  </si>
+  <si>
+    <t>1210118129532018738</t>
+  </si>
+  <si>
+    <t>#YYG92PY8Q</t>
+  </si>
+  <si>
     <t>matanza90</t>
   </si>
   <si>
@@ -815,6 +800,18 @@
   </si>
   <si>
     <t>#GY9UQQY82</t>
+  </si>
+  <si>
+    <t>SirFluffyy</t>
+  </si>
+  <si>
+    <t>sirfluffyy</t>
+  </si>
+  <si>
+    <t>133325280402997248</t>
+  </si>
+  <si>
+    <t>#900088PR9</t>
   </si>
   <si>
     <t>Sned | PST</t>
@@ -1769,17 +1766,23 @@
         <v>65</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1789,19 +1792,19 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>49</v>
@@ -1818,19 +1821,19 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>49</v>
@@ -1847,32 +1850,26 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1882,22 +1879,22 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>15</v>
@@ -1906,7 +1903,7 @@
         <v>16</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1917,26 +1914,32 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1946,32 +1949,26 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -1981,13 +1978,13 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>83</v>
@@ -2005,7 +2002,7 @@
         <v>16</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2025,11 +2022,11 @@
         <v>89</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="F25" s="2" t="s">
         <v>14</v>
       </c>
@@ -2040,7 +2037,7 @@
         <v>16</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2051,26 +2048,32 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="F26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -2080,32 +2083,26 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
@@ -2115,26 +2112,32 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -2144,16 +2147,16 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>104</v>
@@ -2161,15 +2164,9 @@
       <c r="F29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -2181,7 +2178,7 @@
       <c r="A30" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="4" t="s">
         <v>106</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -2273,7 +2270,7 @@
         <v>16</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2308,7 +2305,7 @@
         <v>16</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2363,10 +2360,10 @@
         <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>14</v>
@@ -2389,19 +2386,19 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>14</v>
@@ -2424,26 +2421,32 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
@@ -2453,26 +2456,32 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -2482,26 +2491,32 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
@@ -2511,26 +2526,32 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
@@ -2540,19 +2561,19 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>14</v>
@@ -2564,7 +2585,7 @@
         <v>16</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2575,19 +2596,19 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>14</v>
@@ -2610,32 +2631,26 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
@@ -2654,23 +2669,17 @@
         <v>155</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
@@ -2680,19 +2689,19 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>14</v>
@@ -2715,26 +2724,32 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
+      <c r="G46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
@@ -2744,26 +2759,32 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
+      <c r="G47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
@@ -2773,19 +2794,19 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>14</v>
@@ -2808,19 +2829,19 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>14</v>
@@ -2843,32 +2864,26 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
@@ -2887,23 +2902,17 @@
         <v>180</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
@@ -2913,19 +2922,19 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>14</v>
@@ -2937,7 +2946,7 @@
         <v>16</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -2948,26 +2957,32 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
+      <c r="G53" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
@@ -2977,26 +2992,32 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
+      <c r="G54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
@@ -3006,19 +3027,19 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>14</v>
@@ -3030,7 +3051,7 @@
         <v>16</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -3041,19 +3062,19 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>14</v>
@@ -3065,7 +3086,7 @@
         <v>16</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -3076,32 +3097,26 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
@@ -3111,32 +3126,26 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G58" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
@@ -3146,32 +3155,26 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="D59" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G59" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
@@ -3181,26 +3184,32 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="F60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
+      <c r="G60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
@@ -3210,19 +3219,19 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C61" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="E61" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>14</v>
@@ -3239,16 +3248,16 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>219</v>
@@ -3268,16 +3277,16 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>220</v>
@@ -3285,15 +3294,9 @@
       <c r="F63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G63" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
@@ -3303,13 +3306,13 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>221</v>
@@ -3332,19 +3335,19 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>14</v>
@@ -3361,16 +3364,16 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>225</v>
@@ -3390,13 +3393,13 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>226</v>
@@ -3419,19 +3422,19 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>14</v>
@@ -3448,19 +3451,19 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>14</v>
@@ -3477,16 +3480,16 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>232</v>
@@ -3506,19 +3509,19 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D71" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>14</v>
@@ -3535,19 +3538,19 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D72" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>14</v>
@@ -3564,16 +3567,16 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>237</v>
@@ -3593,19 +3596,19 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>14</v>
@@ -3622,16 +3625,16 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>239</v>
+        <v>209</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>240</v>
@@ -3651,13 +3654,13 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>241</v>
@@ -3680,13 +3683,13 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>243</v>
@@ -3709,26 +3712,32 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>215</v>
+        <v>246</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>216</v>
+        <v>247</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
+      <c r="G78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
@@ -3738,26 +3747,32 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>214</v>
+        <v>249</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>215</v>
+        <v>250</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>216</v>
+        <v>251</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
+      <c r="G79" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
@@ -3767,26 +3782,32 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>215</v>
+        <v>254</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>216</v>
+        <v>255</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
+      <c r="G80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
@@ -3796,19 +3817,19 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>14</v>
@@ -3831,32 +3852,26 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G82" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
@@ -3866,19 +3881,19 @@
     </row>
     <row r="83">
       <c r="A83" s="2" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>14</v>
@@ -3901,22 +3916,22 @@
     </row>
     <row r="84">
       <c r="A84" s="2" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>15</v>
@@ -3925,7 +3940,7 @@
         <v>16</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>28</v>
+        <v>272</v>
       </c>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
@@ -3936,19 +3951,19 @@
     </row>
     <row r="85">
       <c r="A85" s="2" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>14</v>
@@ -3965,32 +3980,26 @@
     </row>
     <row r="86">
       <c r="A86" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="D86" s="2" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>273</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
@@ -4000,19 +4009,19 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="D87" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>14</v>
@@ -4029,26 +4038,32 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
+      <c r="G88" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
@@ -4058,26 +4073,32 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
+      <c r="G89" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
@@ -4087,19 +4108,19 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>14</v>
@@ -4122,19 +4143,19 @@
     </row>
     <row r="91">
       <c r="A91" s="2" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>14</v>
@@ -4146,7 +4167,7 @@
         <v>16</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
@@ -4157,19 +4178,19 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>14</v>
@@ -4181,7 +4202,7 @@
         <v>16</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
@@ -4192,32 +4213,26 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G93" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H93" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I93" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
@@ -4227,32 +4242,26 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>299</v>
-      </c>
       <c r="D94" s="2" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G94" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
@@ -4262,19 +4271,19 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>299</v>
-      </c>
       <c r="D95" s="2" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>14</v>
@@ -4291,19 +4300,19 @@
     </row>
     <row r="96">
       <c r="A96" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>299</v>
-      </c>
       <c r="D96" s="2" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>14</v>
@@ -4320,26 +4329,32 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
+      <c r="G97" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
@@ -4347,77 +4362,13 @@
       <c r="N97" s="3"/>
       <c r="O97" s="3"/>
     </row>
-    <row r="98">
-      <c r="A98" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="3"/>
-      <c r="K98" s="3"/>
-      <c r="L98" s="3"/>
-      <c r="M98" s="3"/>
-      <c r="N98" s="3"/>
-      <c r="O98" s="3"/>
-    </row>
-    <row r="99">
-      <c r="A99" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I99" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J99" s="3"/>
-      <c r="K99" s="3"/>
-      <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
-      <c r="O99" s="3"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:O99">
+  <conditionalFormatting sqref="A2:O97">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:O99">
+  <conditionalFormatting sqref="A2:O97">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
minor changes to lineup algorithm
</commit_message>
<xml_diff>
--- a/xray-members.xlsx
+++ b/xray-members.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="310">
   <si>
     <t>DisplayName</t>
   </si>
@@ -637,21 +637,6 @@
     <t>#2Y88YLL99</t>
   </si>
   <si>
-    <t>CrazyWaveIT | EST</t>
-  </si>
-  <si>
-    <t>crazywaveit</t>
-  </si>
-  <si>
-    <t>642147006776868920</t>
-  </si>
-  <si>
-    <t>CrazyWaveIT</t>
-  </si>
-  <si>
-    <t>#YLUL9Q9JG</t>
-  </si>
-  <si>
     <t>Motz</t>
   </si>
   <si>
@@ -664,15 +649,18 @@
     <t>#G8L8PU8C</t>
   </si>
   <si>
+    <t>Good | EST</t>
+  </si>
+  <si>
+    <t>good0002</t>
+  </si>
+  <si>
+    <t>1168318917014470825</t>
+  </si>
+  <si>
     <t>Good</t>
   </si>
   <si>
-    <t>good0002</t>
-  </si>
-  <si>
-    <t>1168318917014470825</t>
-  </si>
-  <si>
     <t>#QGVR90V0G</t>
   </si>
   <si>
@@ -796,7 +784,7 @@
     <t>Welli</t>
   </si>
   <si>
-    <t>fischusmaximus</t>
+    <t>wellenreiter2006</t>
   </si>
   <si>
     <t>692129916858269736</t>
@@ -2091,9 +2079,15 @@
       <c r="F27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
@@ -3149,11 +3143,11 @@
         <v>210</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="F59" s="2" t="s">
         <v>14</v>
       </c>
@@ -3164,7 +3158,7 @@
         <v>16</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -3175,16 +3169,16 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>216</v>
@@ -3192,15 +3186,9 @@
       <c r="F60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G60" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
@@ -3210,19 +3198,19 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>14</v>
@@ -3239,19 +3227,19 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>14</v>
@@ -3268,26 +3256,32 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="F63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
+      <c r="G63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
@@ -3297,32 +3291,26 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G64" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
@@ -3332,19 +3320,19 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>14</v>
@@ -3361,19 +3349,19 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>14</v>
@@ -3390,19 +3378,19 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>14</v>
@@ -3419,19 +3407,19 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>14</v>
@@ -3448,19 +3436,19 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>14</v>
@@ -3477,19 +3465,19 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>14</v>
@@ -3506,19 +3494,19 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>14</v>
@@ -3535,19 +3523,19 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>236</v>
+        <v>51</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>14</v>
@@ -3564,19 +3552,19 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>51</v>
+        <v>215</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>14</v>
@@ -3593,19 +3581,19 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>14</v>
@@ -3622,19 +3610,19 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>14</v>
@@ -3651,19 +3639,19 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>14</v>
@@ -3680,19 +3668,19 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>14</v>
@@ -3709,19 +3697,19 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>245</v>
+        <v>215</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>14</v>
@@ -3738,19 +3726,19 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>217</v>
+        <v>244</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>14</v>
@@ -3767,19 +3755,19 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>14</v>
@@ -3796,16 +3784,16 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="s">
-        <v>217</v>
+        <v>248</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>218</v>
+        <v>249</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>251</v>
@@ -3813,9 +3801,15 @@
       <c r="F81" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
+      <c r="G81" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
@@ -3939,13 +3933,13 @@
         <v>266</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>15</v>
@@ -3954,7 +3948,7 @@
         <v>16</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>34</v>
+        <v>269</v>
       </c>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
@@ -3965,22 +3959,22 @@
     </row>
     <row r="86">
       <c r="A86" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C86" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="E86" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="E86" s="2" t="s">
-        <v>272</v>
-      </c>
       <c r="F86" s="2" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>15</v>
@@ -3989,7 +3983,7 @@
         <v>16</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>273</v>
+        <v>34</v>
       </c>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
@@ -4000,19 +3994,19 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>14</v>
@@ -4029,19 +4023,19 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>14</v>
@@ -4058,26 +4052,32 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
+      <c r="G89" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
@@ -4087,16 +4087,16 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B90" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>284</v>
@@ -4131,10 +4131,10 @@
         <v>287</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>14</v>
@@ -4157,7 +4157,7 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>290</v>
@@ -4166,11 +4166,11 @@
         <v>291</v>
       </c>
       <c r="D92" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="E92" s="2" t="s">
-        <v>293</v>
-      </c>
       <c r="F92" s="2" t="s">
         <v>14</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>16</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
@@ -4192,7 +4192,7 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>294</v>
@@ -4201,10 +4201,10 @@
         <v>295</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>14</v>
@@ -4216,7 +4216,7 @@
         <v>16</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
@@ -4227,32 +4227,26 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="E94" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="F94" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G94" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
@@ -4262,19 +4256,19 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>14</v>
@@ -4291,19 +4285,19 @@
     </row>
     <row r="96">
       <c r="A96" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>14</v>
@@ -4320,19 +4314,19 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>14</v>
@@ -4349,16 +4343,16 @@
     </row>
     <row r="98">
       <c r="A98" s="2" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>309</v>
@@ -4366,9 +4360,15 @@
       <c r="F98" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
+      <c r="G98" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
@@ -4376,48 +4376,13 @@
       <c r="N98" s="3"/>
       <c r="O98" s="3"/>
     </row>
-    <row r="99">
-      <c r="A99" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I99" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J99" s="3"/>
-      <c r="K99" s="3"/>
-      <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
-      <c r="O99" s="3"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:O99">
+  <conditionalFormatting sqref="A2:O98">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:O99">
+  <conditionalFormatting sqref="A2:O98">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
update strikes + blacklist
</commit_message>
<xml_diff>
--- a/xray-members.xlsx
+++ b/xray-members.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="332">
   <si>
     <t>DisplayName</t>
   </si>
@@ -73,6 +73,9 @@
     <t>#2PCJ8RVYG</t>
   </si>
   <si>
+    <t>Mem</t>
+  </si>
+  <si>
     <t>Sugma</t>
   </si>
   <si>
@@ -115,9 +118,6 @@
     <t>#92L2PP09R</t>
   </si>
   <si>
-    <t>Mem</t>
-  </si>
-  <si>
     <t>Mini @ñ@$</t>
   </si>
   <si>
@@ -331,18 +331,6 @@
     <t>#99Q0R0YQ9</t>
   </si>
   <si>
-    <t>Az7777</t>
-  </si>
-  <si>
-    <t>11111111111764</t>
-  </si>
-  <si>
-    <t>852669877407711272</t>
-  </si>
-  <si>
-    <t>#QYLURLQ2</t>
-  </si>
-  <si>
     <t>Dalto</t>
   </si>
   <si>
@@ -439,15 +427,6 @@
     <t>#PG2Y8RGU</t>
   </si>
   <si>
-    <t>appable</t>
-  </si>
-  <si>
-    <t>529061226819485727</t>
-  </si>
-  <si>
-    <t>#CVYG8LU</t>
-  </si>
-  <si>
     <t>Carsonn</t>
   </si>
   <si>
@@ -538,6 +517,30 @@
     <t>#RV920PR9</t>
   </si>
   <si>
+    <t>Sphinx</t>
+  </si>
+  <si>
+    <t>sinofgreed5085</t>
+  </si>
+  <si>
+    <t>383151051425054731</t>
+  </si>
+  <si>
+    <t>Sin Of Greed</t>
+  </si>
+  <si>
+    <t>#9PR280J8J</t>
+  </si>
+  <si>
+    <t>AMIXUS 2</t>
+  </si>
+  <si>
+    <t>#9VVYGPUQP</t>
+  </si>
+  <si>
+    <t>#P8VUQU0RJ</t>
+  </si>
+  <si>
     <t>Marlec | CEST</t>
   </si>
   <si>
@@ -569,6 +572,69 @@
   </si>
   <si>
     <t>#LVQ9PPQVY</t>
+  </si>
+  <si>
+    <t>Selug</t>
+  </si>
+  <si>
+    <t>#G99UVRLU0</t>
+  </si>
+  <si>
+    <t>jovc</t>
+  </si>
+  <si>
+    <t>#QJL2UG902</t>
+  </si>
+  <si>
+    <t>timi bää 7</t>
+  </si>
+  <si>
+    <t>#G02PPURRQ</t>
+  </si>
+  <si>
+    <t>Marlec9207</t>
+  </si>
+  <si>
+    <t>#P8QYVVV2J</t>
+  </si>
+  <si>
+    <t>Houdi</t>
+  </si>
+  <si>
+    <t>#PPPUUUQ20</t>
+  </si>
+  <si>
+    <t>BU$HI</t>
+  </si>
+  <si>
+    <t>#G29YQ8VUP</t>
+  </si>
+  <si>
+    <t>SDM</t>
+  </si>
+  <si>
+    <t>#L0RL9RP0Y</t>
+  </si>
+  <si>
+    <t>Luther</t>
+  </si>
+  <si>
+    <t>#L822V0G9L</t>
+  </si>
+  <si>
+    <t>CrazyWaveIT | EST</t>
+  </si>
+  <si>
+    <t>terntenodo</t>
+  </si>
+  <si>
+    <t>485310245929877534</t>
+  </si>
+  <si>
+    <t>CrazyWaveIT</t>
+  </si>
+  <si>
+    <t>#YLUL9Q9JG</t>
   </si>
   <si>
     <t>Ascended | IST</t>
@@ -980,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -991,9 +1057,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1323,9 +1386,15 @@
       <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -1344,10 +1413,10 @@
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>14</v>
@@ -1373,10 +1442,10 @@
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>14</v>
@@ -1393,19 +1462,19 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>14</v>
@@ -1428,19 +1497,19 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>14</v>
@@ -1452,7 +1521,7 @@
         <v>16</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1463,13 +1532,13 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>35</v>
@@ -1492,13 +1561,13 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>37</v>
@@ -1545,7 +1614,7 @@
         <v>16</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1754,7 +1823,7 @@
         <v>16</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1789,7 +1858,7 @@
         <v>16</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1853,7 +1922,7 @@
         <v>16</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1981,7 +2050,7 @@
         <v>16</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2051,7 +2120,7 @@
         <v>16</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2086,7 +2155,7 @@
         <v>16</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2112,7 +2181,7 @@
         <v>99</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>15</v>
@@ -2185,7 +2254,7 @@
         <v>16</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2198,7 +2267,7 @@
       <c r="A31" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>107</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -2220,7 +2289,7 @@
         <v>16</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2255,7 +2324,7 @@
         <v>16</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2290,7 +2359,7 @@
         <v>16</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2325,7 +2394,7 @@
         <v>16</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2360,7 +2429,7 @@
         <v>16</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2380,10 +2449,10 @@
         <v>128</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>14</v>
@@ -2395,7 +2464,7 @@
         <v>16</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2406,16 +2475,16 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>134</v>
@@ -2430,7 +2499,7 @@
         <v>16</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2444,16 +2513,16 @@
         <v>135</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>14</v>
@@ -2465,7 +2534,7 @@
         <v>16</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -2476,7 +2545,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>139</v>
@@ -2485,7 +2554,7 @@
         <v>140</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>141</v>
@@ -2500,7 +2569,7 @@
         <v>16</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -2514,16 +2583,16 @@
         <v>142</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>14</v>
@@ -2535,7 +2604,7 @@
         <v>16</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -2546,19 +2615,19 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>14</v>
@@ -2570,7 +2639,7 @@
         <v>16</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2581,13 +2650,13 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>152</v>
@@ -2598,15 +2667,9 @@
       <c r="F42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
@@ -2616,32 +2679,26 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="F43" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
@@ -2651,26 +2708,32 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="F44" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
+      <c r="G44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
@@ -2680,26 +2743,32 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
+      <c r="G45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
@@ -2709,19 +2778,19 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="E46" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>14</v>
@@ -2733,7 +2802,7 @@
         <v>16</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -2744,32 +2813,26 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
@@ -2779,16 +2842,16 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>174</v>
@@ -2796,15 +2859,9 @@
       <c r="F48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
@@ -2814,26 +2871,32 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>179</v>
-      </c>
       <c r="F49" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
+      <c r="G49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
@@ -2843,19 +2906,19 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>14</v>
@@ -2872,19 +2935,19 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>14</v>
@@ -2901,32 +2964,26 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="F52" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G52" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
@@ -2936,20 +2993,20 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="F53" s="2" t="s">
         <v>14</v>
       </c>
@@ -2960,7 +3017,7 @@
         <v>16</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -2971,19 +3028,19 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>14</v>
@@ -3000,19 +3057,19 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>14</v>
@@ -3029,32 +3086,26 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G56" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
@@ -3064,32 +3115,26 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
@@ -3099,32 +3144,26 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G58" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
@@ -3134,32 +3173,26 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G59" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
@@ -3169,19 +3202,19 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>14</v>
@@ -3198,19 +3231,19 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>14</v>
@@ -3227,26 +3260,32 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
@@ -3256,20 +3295,20 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="F63" s="2" t="s">
         <v>14</v>
       </c>
@@ -3280,7 +3319,7 @@
         <v>16</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -3291,19 +3330,19 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>14</v>
@@ -3320,19 +3359,19 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>14</v>
@@ -3349,26 +3388,32 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
+      <c r="G66" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
@@ -3378,26 +3423,32 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="D67" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="F67" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
+      <c r="G67" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
@@ -3407,26 +3458,32 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
+      <c r="G68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
@@ -3436,26 +3493,32 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
+      <c r="G69" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
@@ -3465,19 +3528,19 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>14</v>
@@ -3494,19 +3557,19 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>14</v>
@@ -3523,19 +3586,19 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>51</v>
+        <v>237</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>14</v>
@@ -3552,26 +3615,32 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
+      <c r="G73" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
@@ -3581,19 +3650,19 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>14</v>
@@ -3610,19 +3679,19 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>14</v>
@@ -3639,19 +3708,19 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>14</v>
@@ -3668,19 +3737,19 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>14</v>
@@ -3697,19 +3766,19 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>14</v>
@@ -3726,19 +3795,19 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>14</v>
@@ -3755,19 +3824,19 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>14</v>
@@ -3784,32 +3853,26 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G81" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I81" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
@@ -3819,32 +3882,26 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>252</v>
+        <v>51</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G82" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
@@ -3854,32 +3911,26 @@
     </row>
     <row r="83">
       <c r="A83" s="2" t="s">
-        <v>256</v>
+        <v>234</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="F83" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G83" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
@@ -3889,32 +3940,26 @@
     </row>
     <row r="84">
       <c r="A84" s="2" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G84" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
@@ -3924,32 +3969,26 @@
     </row>
     <row r="85">
       <c r="A85" s="2" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>269</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
@@ -3959,32 +3998,26 @@
     </row>
     <row r="86">
       <c r="A86" s="2" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G86" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
@@ -3994,19 +4027,19 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>273</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>14</v>
@@ -4023,19 +4056,19 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>275</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>14</v>
@@ -4052,32 +4085,26 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="s">
-        <v>276</v>
+        <v>234</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>277</v>
+        <v>235</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>278</v>
+        <v>236</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G89" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I89" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
@@ -4087,32 +4114,26 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="s">
-        <v>281</v>
+        <v>234</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>282</v>
+        <v>235</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>283</v>
+        <v>236</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G90" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H90" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
@@ -4122,19 +4143,19 @@
     </row>
     <row r="91">
       <c r="A91" s="2" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>14</v>
@@ -4146,7 +4167,7 @@
         <v>16</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
@@ -4157,19 +4178,19 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>14</v>
@@ -4181,7 +4202,7 @@
         <v>16</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
@@ -4192,19 +4213,19 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>14</v>
@@ -4216,7 +4237,7 @@
         <v>16</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
@@ -4227,26 +4248,32 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
+      <c r="G94" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
@@ -4256,26 +4283,32 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
-      <c r="I95" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>291</v>
+      </c>
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
       <c r="L95" s="3"/>
@@ -4285,26 +4318,32 @@
     </row>
     <row r="96">
       <c r="A96" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E96" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>303</v>
-      </c>
       <c r="F96" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
+      <c r="G96" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
@@ -4314,19 +4353,19 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B97" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="E97" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>14</v>
@@ -4343,32 +4382,26 @@
     </row>
     <row r="98">
       <c r="A98" s="2" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G98" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
@@ -4376,13 +4409,339 @@
       <c r="N98" s="3"/>
       <c r="O98" s="3"/>
     </row>
+    <row r="99">
+      <c r="A99" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J99" s="3"/>
+      <c r="K99" s="3"/>
+      <c r="L99" s="3"/>
+      <c r="M99" s="3"/>
+      <c r="N99" s="3"/>
+      <c r="O99" s="3"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="3"/>
+      <c r="M100" s="3"/>
+      <c r="N100" s="3"/>
+      <c r="O100" s="3"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
+      <c r="M101" s="3"/>
+      <c r="N101" s="3"/>
+      <c r="O101" s="3"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+      <c r="M102" s="3"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="3"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+      <c r="M103" s="3"/>
+      <c r="N103" s="3"/>
+      <c r="O103" s="3"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+      <c r="M104" s="3"/>
+      <c r="N104" s="3"/>
+      <c r="O104" s="3"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+      <c r="M105" s="3"/>
+      <c r="N105" s="3"/>
+      <c r="O105" s="3"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="3"/>
+      <c r="N106" s="3"/>
+      <c r="O106" s="3"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="3"/>
+      <c r="M107" s="3"/>
+      <c r="N107" s="3"/>
+      <c r="O107" s="3"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:O98">
+  <conditionalFormatting sqref="A2:O108">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:O98">
+  <conditionalFormatting sqref="A2:O108">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>